<commit_message>
Fix import dan menghilangkan  total potongan dan total tunjangan
</commit_message>
<xml_diff>
--- a/asset/file/DATA TRANSPORT DAN POTONGAN.xlsx
+++ b/asset/file/DATA TRANSPORT DAN POTONGAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\penggajian\asset\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F5EE01-1B60-41B8-A3A6-7C507E1AA516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCC0363-C7B0-4930-A347-897CA3472D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6CAE5FFD-6662-41DA-B693-4965D4BC20C9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>DATA GUKAR</t>
   </si>
@@ -99,9 +99,6 @@
     <t>TABUNGAN QURBAN</t>
   </si>
   <si>
-    <t>TOTAL POTONGAN</t>
-  </si>
-  <si>
     <t>TUNJANGAN ANAK</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
   </si>
   <si>
     <t>Kabid BKK</t>
-  </si>
-  <si>
-    <t>TOTAL TUNJANGAN</t>
   </si>
   <si>
     <t>BPJS</t>
@@ -613,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C141464D-BD7B-4BCF-9FF6-395CBA6AAE97}">
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,13 +634,11 @@
     <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -673,10 +665,8 @@
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
       <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
     </row>
-    <row r="2" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -696,7 +686,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>7</v>
@@ -749,28 +739,22 @@
       <c r="X2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="B3" s="4">
         <v>1234</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="F3" s="5">
         <v>100000</v>
@@ -821,7 +805,7 @@
         <v>45000</v>
       </c>
       <c r="V3" s="6">
-        <v>675000</v>
+        <v>45000</v>
       </c>
       <c r="W3" s="6">
         <v>45000</v>
@@ -829,28 +813,22 @@
       <c r="X3" s="6">
         <v>45000</v>
       </c>
-      <c r="Y3" s="6">
-        <v>45000</v>
-      </c>
-      <c r="Z3" s="6">
-        <v>135000</v>
-      </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4">
         <v>331006</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="5">
         <v>100000</v>
@@ -901,7 +879,7 @@
         <v>45000</v>
       </c>
       <c r="V4" s="6">
-        <v>675000</v>
+        <v>45000</v>
       </c>
       <c r="W4" s="6">
         <v>45000</v>
@@ -909,28 +887,22 @@
       <c r="X4" s="6">
         <v>45000</v>
       </c>
-      <c r="Y4" s="6">
-        <v>45000</v>
-      </c>
-      <c r="Z4" s="6">
-        <v>135000</v>
-      </c>
     </row>
-    <row r="5" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4">
         <v>838656</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="5">
         <v>100000</v>
@@ -981,7 +953,7 @@
         <v>45000</v>
       </c>
       <c r="V5" s="6">
-        <v>675000</v>
+        <v>45000</v>
       </c>
       <c r="W5" s="6">
         <v>45000</v>
@@ -989,28 +961,22 @@
       <c r="X5" s="6">
         <v>45000</v>
       </c>
-      <c r="Y5" s="6">
-        <v>45000</v>
-      </c>
-      <c r="Z5" s="6">
-        <v>135000</v>
-      </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4">
         <v>1188171</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5">
         <v>100000</v>
@@ -1061,7 +1027,7 @@
         <v>45000</v>
       </c>
       <c r="V6" s="6">
-        <v>675000</v>
+        <v>45000</v>
       </c>
       <c r="W6" s="6">
         <v>45000</v>
@@ -1069,28 +1035,22 @@
       <c r="X6" s="6">
         <v>45000</v>
       </c>
-      <c r="Y6" s="6">
-        <v>45000</v>
-      </c>
-      <c r="Z6" s="6">
-        <v>135000</v>
-      </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4">
         <v>1034905</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="5">
         <v>100000</v>
@@ -1141,24 +1101,18 @@
         <v>45000</v>
       </c>
       <c r="V7" s="6">
-        <v>675000</v>
+        <v>45000</v>
       </c>
       <c r="W7" s="6">
         <v>45000</v>
       </c>
       <c r="X7" s="6">
         <v>45000</v>
-      </c>
-      <c r="Y7" s="6">
-        <v>45000</v>
-      </c>
-      <c r="Z7" s="6">
-        <v>135000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>